<commit_message>
node-express-mongodb updated to v.1.1.4
</commit_message>
<xml_diff>
--- a/data_sheets/new-york.xlsx
+++ b/data_sheets/new-york.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\tubemaphistory\tube-map-history.api\data_sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E54C4E83-8CD9-4489-A973-879E80291C4E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C398A34-76BD-4EBD-9FB2-34861622E7A7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8472" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Stations" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="37">
   <si>
     <t>name</t>
   </si>
@@ -126,6 +126,12 @@
   </si>
   <si>
     <t>BMT Broadway Line</t>
+  </si>
+  <si>
+    <t>key</t>
+  </si>
+  <si>
+    <t>BMT Broadway</t>
   </si>
 </sst>
 </file>
@@ -764,80 +770,83 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52BDE343-72F3-4832-82E9-A2F8F0EAFC0D}">
-  <dimension ref="A1:K18"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="8" max="8" width="26.19921875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="29.796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="26.19921875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="29.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>21</v>
       </c>
       <c r="B1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>22</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>23</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>24</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>25</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>26</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>27</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>28</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>29</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" t="s">
         <v>34</v>
       </c>
-      <c r="C2" t="s">
-        <v>31</v>
-      </c>
       <c r="D2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" t="s">
         <v>32</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>33</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>1917</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>26</v>
       </c>
-      <c r="B4" t="s">
-        <v>26</v>
-      </c>
       <c r="C4" t="s">
         <v>26</v>
       </c>
@@ -854,124 +863,127 @@
         <v>26</v>
       </c>
       <c r="H4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I4" t="s">
         <v>16</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>15</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>1919</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I5" t="s">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J5" t="s">
         <v>10</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>1919</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I6" t="s">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J6" t="s">
         <v>9</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>1919</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I7" t="s">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J7" t="s">
         <v>19</v>
       </c>
-      <c r="J7">
-        <v>1918</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I8" t="s">
+      <c r="K7">
+        <v>1918</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J8" t="s">
         <v>8</v>
       </c>
-      <c r="J8">
-        <v>1918</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I9" t="s">
+      <c r="K8">
+        <v>1918</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J9" t="s">
         <v>7</v>
       </c>
-      <c r="J9">
-        <v>1918</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I10" t="s">
+      <c r="K9">
+        <v>1918</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J10" t="s">
         <v>6</v>
       </c>
-      <c r="J10">
-        <v>1918</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I11" t="s">
+      <c r="K10">
+        <v>1918</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J11" t="s">
         <v>5</v>
       </c>
-      <c r="J11">
+      <c r="K11">
         <v>1917</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I12" t="s">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J12" t="s">
         <v>14</v>
       </c>
-      <c r="J12">
+      <c r="K12">
         <v>1917</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I13" t="s">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J13" t="s">
         <v>17</v>
       </c>
-      <c r="J13">
+      <c r="K13">
         <v>1917</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I14" t="s">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J14" t="s">
         <v>11</v>
       </c>
-      <c r="J14">
+      <c r="K14">
         <v>1917</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I15" t="s">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J15" t="s">
         <v>12</v>
       </c>
-      <c r="J15">
-        <v>1918</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="I16" t="s">
+      <c r="K15">
+        <v>1918</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="J16" t="s">
         <v>13</v>
       </c>
-      <c r="J16">
-        <v>1918</v>
-      </c>
-    </row>
-    <row r="17" spans="9:10" x14ac:dyDescent="0.3">
-      <c r="I17" t="s">
+      <c r="K16">
+        <v>1918</v>
+      </c>
+    </row>
+    <row r="17" spans="10:11" x14ac:dyDescent="0.3">
+      <c r="J17" t="s">
         <v>18</v>
       </c>
-      <c r="J17">
-        <v>1918</v>
-      </c>
-    </row>
-    <row r="18" spans="9:10" x14ac:dyDescent="0.3">
-      <c r="I18" t="s">
+      <c r="K17">
+        <v>1918</v>
+      </c>
+    </row>
+    <row r="18" spans="10:11" x14ac:dyDescent="0.3">
+      <c r="J18" t="s">
         <v>20</v>
       </c>
-      <c r="J18">
+      <c r="K18">
         <v>1918</v>
       </c>
     </row>

</xml_diff>